<commit_message>
ADD A N, ADD A (HL), ADC A N, ADC A (HL), SUB A N, SUB A (HL), SBC A N, SBC A (HL)
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -845,24 +845,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1118,515 +1122,515 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="str">
+      <c r="B1" s="1" t="str">
         <f aca="false">DEC2HEX(0, 2)</f>
         <v>00</v>
       </c>
-      <c r="C1" s="0" t="str">
+      <c r="C1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(B1)+1, 2)</f>
         <v>01</v>
       </c>
-      <c r="D1" s="0" t="str">
+      <c r="D1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(C1)+1, 2)</f>
         <v>02</v>
       </c>
-      <c r="E1" s="0" t="str">
+      <c r="E1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(D1)+1, 2)</f>
         <v>03</v>
       </c>
-      <c r="F1" s="0" t="str">
+      <c r="F1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(E1)+1, 2)</f>
         <v>04</v>
       </c>
-      <c r="G1" s="0" t="str">
+      <c r="G1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(F1)+1, 2)</f>
         <v>05</v>
       </c>
-      <c r="H1" s="0" t="str">
+      <c r="H1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(G1)+1, 2)</f>
         <v>06</v>
       </c>
-      <c r="I1" s="0" t="str">
+      <c r="I1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(H1)+1, 2)</f>
         <v>07</v>
       </c>
-      <c r="J1" s="0" t="str">
+      <c r="J1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(I1)+1, 2)</f>
         <v>08</v>
       </c>
-      <c r="K1" s="0" t="str">
+      <c r="K1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(J1)+1, 2)</f>
         <v>09</v>
       </c>
-      <c r="L1" s="0" t="str">
+      <c r="L1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(K1)+1, 2)</f>
         <v>0A</v>
       </c>
-      <c r="M1" s="0" t="str">
+      <c r="M1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(L1)+1, 2)</f>
         <v>0B</v>
       </c>
-      <c r="N1" s="0" t="str">
+      <c r="N1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(M1)+1, 2)</f>
         <v>0C</v>
       </c>
-      <c r="O1" s="0" t="str">
+      <c r="O1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(N1)+1, 2)</f>
         <v>0D</v>
       </c>
-      <c r="P1" s="0" t="str">
+      <c r="P1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(O1)+1, 2)</f>
         <v>0E</v>
       </c>
-      <c r="Q1" s="0" t="str">
+      <c r="Q1" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(P1)+1, 2)</f>
         <v>0F</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
+      <c r="A2" s="1" t="str">
         <f aca="false">DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
+      <c r="A3" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A2)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
+      <c r="A4" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A3)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
+      <c r="A5" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A4)+16, 2)</f>
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="str">
+      <c r="A6" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A5)+16, 2)</f>
         <v>40</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="str">
+      <c r="A7" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A6)+16, 2)</f>
         <v>50</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="str">
+      <c r="A8" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A7)+16, 2)</f>
         <v>60</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="str">
+      <c r="A9" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A8)+16, 2)</f>
         <v>70</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="str">
+      <c r="A10" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A9)+16, 2)</f>
         <v>80</v>
       </c>
@@ -1680,7 +1684,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="str">
+      <c r="A11" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A10)+16, 2)</f>
         <v>90</v>
       </c>
@@ -1734,724 +1738,724 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="str">
+      <c r="A12" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A11)+16, 2)</f>
         <v>A0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="str">
+      <c r="A13" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A12)+16, 2)</f>
         <v>B0</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="str">
+      <c r="A14" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A13)+16, 2)</f>
         <v>C0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="str">
+      <c r="A15" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A14)+16, 2)</f>
         <v>D0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2" t="s">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2" t="s">
+      <c r="O15" s="3"/>
+      <c r="P15" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="str">
+      <c r="A16" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A15)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2" t="s">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="str">
+      <c r="A17" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A16)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2" t="s">
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q17" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="str">
+      <c r="B20" s="1" t="str">
         <f aca="false">DEC2HEX(0, 2)</f>
         <v>00</v>
       </c>
-      <c r="C20" s="0" t="str">
+      <c r="C20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(B20)+1, 2)</f>
         <v>01</v>
       </c>
-      <c r="D20" s="0" t="str">
+      <c r="D20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(C20)+1, 2)</f>
         <v>02</v>
       </c>
-      <c r="E20" s="0" t="str">
+      <c r="E20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(D20)+1, 2)</f>
         <v>03</v>
       </c>
-      <c r="F20" s="0" t="str">
+      <c r="F20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(E20)+1, 2)</f>
         <v>04</v>
       </c>
-      <c r="G20" s="0" t="str">
+      <c r="G20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(F20)+1, 2)</f>
         <v>05</v>
       </c>
-      <c r="H20" s="0" t="str">
+      <c r="H20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(G20)+1, 2)</f>
         <v>06</v>
       </c>
-      <c r="I20" s="0" t="str">
+      <c r="I20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(H20)+1, 2)</f>
         <v>07</v>
       </c>
-      <c r="J20" s="0" t="str">
+      <c r="J20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(I20)+1, 2)</f>
         <v>08</v>
       </c>
-      <c r="K20" s="0" t="str">
+      <c r="K20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(J20)+1, 2)</f>
         <v>09</v>
       </c>
-      <c r="L20" s="0" t="str">
+      <c r="L20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(K20)+1, 2)</f>
         <v>0A</v>
       </c>
-      <c r="M20" s="0" t="str">
+      <c r="M20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(L20)+1, 2)</f>
         <v>0B</v>
       </c>
-      <c r="N20" s="0" t="str">
+      <c r="N20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(M20)+1, 2)</f>
         <v>0C</v>
       </c>
-      <c r="O20" s="0" t="str">
+      <c r="O20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(N20)+1, 2)</f>
         <v>0D</v>
       </c>
-      <c r="P20" s="0" t="str">
+      <c r="P20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(O20)+1, 2)</f>
         <v>0E</v>
       </c>
-      <c r="Q20" s="0" t="str">
+      <c r="Q20" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(P20)+1, 2)</f>
         <v>0F</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="str">
+      <c r="A21" s="1" t="str">
         <f aca="false">DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="str">
+      <c r="A22" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A21)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="str">
+      <c r="A23" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A22)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="str">
+      <c r="A24" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A23)+16, 2)</f>
         <v>30</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="str">
+      <c r="A25" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A24)+16, 2)</f>
         <v>40</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="str">
+      <c r="A26" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A25)+16, 2)</f>
         <v>50</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="str">
+      <c r="A27" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A26)+16, 2)</f>
         <v>60</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="str">
+      <c r="A28" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A27)+16, 2)</f>
         <v>70</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="str">
+      <c r="A29" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A28)+16, 2)</f>
         <v>80</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="str">
+      <c r="A30" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A29)+16, 2)</f>
         <v>90</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="str">
+      <c r="A31" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A30)+16, 2)</f>
         <v>A0</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="str">
+      <c r="A32" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A31)+16, 2)</f>
         <v>B0</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="str">
+      <c r="A33" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A32)+16, 2)</f>
         <v>C0</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="str">
+      <c r="A34" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A33)+16, 2)</f>
         <v>D0</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="str">
+      <c r="A35" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A34)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="str">
+      <c r="A36" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A35)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
AND A N, AND A (HL), XOR A N, XOR A (HL), OR A N, OR A (HL), CP A N, CP A (HL)
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
+      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1742,52 +1742,52 @@
         <f aca="false">DEC2HEX(HEX2DEC(A11)+16, 2)</f>
         <v>A0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="Q12" s="2" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1796,52 +1796,52 @@
         <f aca="false">DEC2HEX(HEX2DEC(A12)+16, 2)</f>
         <v>B0</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="Q13" s="2" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PUSH NN, POP NN, bus latching/open bus, timing updates to (HL) opcodes
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -766,7 +766,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,6 +789,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -799,8 +806,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2A1"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF395511"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
   </fills>
@@ -845,7 +852,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -854,15 +861,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -916,7 +927,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFE8F2A1"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -932,7 +943,7 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF395511"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -1122,7 +1133,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1132,910 +1143,911 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="str">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="str">
         <f aca="false">DEC2HEX(0, 2)</f>
         <v>00</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(B1)+1, 2)</f>
         <v>01</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(C1)+1, 2)</f>
         <v>02</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="E1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(D1)+1, 2)</f>
         <v>03</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="F1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(E1)+1, 2)</f>
         <v>04</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="G1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(F1)+1, 2)</f>
         <v>05</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="H1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(G1)+1, 2)</f>
         <v>06</v>
       </c>
-      <c r="I1" s="1" t="str">
+      <c r="I1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(H1)+1, 2)</f>
         <v>07</v>
       </c>
-      <c r="J1" s="1" t="str">
+      <c r="J1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(I1)+1, 2)</f>
         <v>08</v>
       </c>
-      <c r="K1" s="1" t="str">
+      <c r="K1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(J1)+1, 2)</f>
         <v>09</v>
       </c>
-      <c r="L1" s="1" t="str">
+      <c r="L1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(K1)+1, 2)</f>
         <v>0A</v>
       </c>
-      <c r="M1" s="1" t="str">
+      <c r="M1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(L1)+1, 2)</f>
         <v>0B</v>
       </c>
-      <c r="N1" s="1" t="str">
+      <c r="N1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(M1)+1, 2)</f>
         <v>0C</v>
       </c>
-      <c r="O1" s="1" t="str">
+      <c r="O1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(N1)+1, 2)</f>
         <v>0D</v>
       </c>
-      <c r="P1" s="1" t="str">
+      <c r="P1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(O1)+1, 2)</f>
         <v>0E</v>
       </c>
-      <c r="Q1" s="1" t="str">
+      <c r="Q1" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(P1)+1, 2)</f>
         <v>0F</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="str">
+      <c r="A2" s="2" t="str">
         <f aca="false">DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="str">
+      <c r="A3" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A2)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="str">
+      <c r="A4" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A3)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="str">
+      <c r="A5" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A4)+16, 2)</f>
         <v>30</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="str">
+      <c r="A6" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A5)+16, 2)</f>
         <v>40</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="str">
+      <c r="A7" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A6)+16, 2)</f>
         <v>50</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="str">
+      <c r="A8" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A7)+16, 2)</f>
         <v>60</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="str">
+      <c r="A9" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A8)+16, 2)</f>
         <v>70</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="str">
+      <c r="A10" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A9)+16, 2)</f>
         <v>80</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N10" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="str">
+      <c r="A11" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A10)+16, 2)</f>
         <v>90</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="str">
+      <c r="A12" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A11)+16, 2)</f>
         <v>A0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="str">
+      <c r="A13" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A12)+16, 2)</f>
         <v>B0</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="str">
+      <c r="A14" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A13)+16, 2)</f>
         <v>C0</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>192</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>196</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="str">
+      <c r="A15" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A14)+16, 2)</f>
         <v>D0</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>208</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>211</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3" t="s">
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3" t="s">
+      <c r="O15" s="4"/>
+      <c r="P15" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="Q15" s="4" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="str">
+      <c r="A16" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A15)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>221</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3" t="s">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q16" s="4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="str">
+      <c r="A17" s="2" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A16)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>232</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3" t="s">
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="Q17" s="3" t="s">
+      <c r="Q17" s="4" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2110,352 +2122,352 @@
         <f aca="false">DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A21)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A22)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A23)+16, 2)</f>
         <v>30</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A24)+16, 2)</f>
         <v>40</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A25)+16, 2)</f>
         <v>50</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A26)+16, 2)</f>
         <v>60</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A27)+16, 2)</f>
         <v>70</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A28)+16, 2)</f>
         <v>80</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A29)+16, 2)</f>
         <v>90</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A30)+16, 2)</f>
         <v>A0</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A31)+16, 2)</f>
         <v>B0</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A32)+16, 2)</f>
         <v>C0</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A33)+16, 2)</f>
         <v>D0</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A34)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A35)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
RET, RET F, RETI, LDH A A8, LDH A8 A, LD NN N16
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1217,7 +1217,7 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1271,7 +1271,7 @@
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1325,7 +1325,7 @@
       <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1379,7 +1379,7 @@
       <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1862,7 +1862,7 @@
         <f aca="false">DEC2HEX(HEX2DEC(A13)+16, 2)</f>
         <v>C0</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>192</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1886,10 +1886,10 @@
       <c r="I14" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>201</v>
       </c>
       <c r="L14" s="4" t="s">
@@ -1916,7 +1916,7 @@
         <f aca="false">DEC2HEX(HEX2DEC(A14)+16, 2)</f>
         <v>D0</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>208</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1938,10 +1938,10 @@
       <c r="I15" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>216</v>
       </c>
       <c r="L15" s="4" t="s">
@@ -1964,7 +1964,7 @@
         <f aca="false">DEC2HEX(HEX2DEC(A15)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>221</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -2008,7 +2008,7 @@
         <f aca="false">DEC2HEX(HEX2DEC(A16)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>232</v>
       </c>
       <c r="C17" s="3" t="s">

</xml_diff>

<commit_message>
LD NN A, LD HLD A, LD HLI A, LD A NN, LD A HLD, LD A HLI, JP, JP F, LDH A8 A, LDH A A8
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
+      <selection pane="topLeft" activeCell="U13" activeCellId="0" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1220,7 +1220,7 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1244,7 +1244,7 @@
       <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -1274,7 +1274,7 @@
       <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1298,7 +1298,7 @@
       <c r="K3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -1328,7 +1328,7 @@
       <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1352,7 +1352,7 @@
       <c r="K4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -1382,7 +1382,7 @@
       <c r="C5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1406,7 +1406,7 @@
       <c r="K5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>58</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -1868,10 +1868,10 @@
       <c r="C14" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>195</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1892,7 +1892,7 @@
       <c r="K14" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>202</v>
       </c>
       <c r="M14" s="5" t="s">
@@ -1922,7 +1922,7 @@
       <c r="C15" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>210</v>
       </c>
       <c r="E15" s="4"/>
@@ -1944,7 +1944,7 @@
       <c r="K15" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="3" t="s">
         <v>217</v>
       </c>
       <c r="M15" s="4"/>
@@ -1970,7 +1970,7 @@
       <c r="C16" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>223</v>
       </c>
       <c r="E16" s="4"/>
@@ -2014,7 +2014,7 @@
       <c r="C17" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>234</v>
       </c>
       <c r="E17" s="4" t="s">

</xml_diff>

<commit_message>
INC NN, DEC NN, Invalid, EI, DI, STOP, HALT
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U13" activeCellId="0" sqref="U13"/>
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1223,7 +1223,7 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1247,7 +1247,7 @@
       <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="4" t="s">
@@ -1268,7 +1268,7 @@
         <f aca="false">DEC2HEX(HEX2DEC(A2)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1277,7 +1277,7 @@
       <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1301,7 +1301,7 @@
       <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="4" t="s">
@@ -1331,7 +1331,7 @@
       <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1355,7 +1355,7 @@
       <c r="L4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>43</v>
       </c>
       <c r="N4" s="4" t="s">
@@ -1385,7 +1385,7 @@
       <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1409,7 +1409,7 @@
       <c r="L5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>59</v>
       </c>
       <c r="N5" s="4" t="s">
@@ -1610,7 +1610,7 @@
       <c r="G9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>118</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -1925,7 +1925,7 @@
       <c r="D15" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="4" t="s">
         <v>211</v>
       </c>
@@ -1947,11 +1947,11 @@
       <c r="L15" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="O15" s="4"/>
+      <c r="O15" s="3"/>
       <c r="P15" s="4" t="s">
         <v>219</v>
       </c>
@@ -1973,8 +1973,8 @@
       <c r="D16" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>224</v>
       </c>
@@ -1993,9 +1993,9 @@
       <c r="L16" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
       <c r="P16" s="4" t="s">
         <v>230</v>
       </c>
@@ -2017,10 +2017,10 @@
       <c r="D17" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
         <v>236</v>
       </c>
@@ -2039,11 +2039,11 @@
       <c r="L17" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
       <c r="P17" s="4" t="s">
         <v>243</v>
       </c>

</xml_diff>

<commit_message>
INC N, DEC N, CALL, CALL F
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
+      <selection pane="topLeft" activeCell="V9" activeCellId="0" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1226,10 +1226,10 @@
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -1250,10 +1250,10 @@
       <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -1280,10 +1280,10 @@
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -1304,10 +1304,10 @@
       <c r="M3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="4" t="s">
@@ -1334,10 +1334,10 @@
       <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -1358,10 +1358,10 @@
       <c r="M4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -1388,10 +1388,10 @@
       <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1412,10 +1412,10 @@
       <c r="M5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="3" t="s">
         <v>61</v>
       </c>
       <c r="P5" s="4" t="s">
@@ -1874,7 +1874,7 @@
       <c r="E14" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>196</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1898,10 +1898,10 @@
       <c r="M14" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N14" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="3" t="s">
         <v>205</v>
       </c>
       <c r="P14" s="4" t="s">
@@ -1926,7 +1926,7 @@
         <v>210</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>211</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1948,7 +1948,7 @@
         <v>217</v>
       </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="3" t="s">
         <v>218</v>
       </c>
       <c r="O15" s="3"/>

</xml_diff>

<commit_message>
ADD A N8, ADC A N8, SUB A N8, SBC A N8, AND A N8, XOR A N8, OR A N8, CP A N8, RLCA, RLA, RRCA, RRA, DAA, SCF, CCF, CPL
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V9" activeCellId="0" sqref="V9"/>
+      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1232,10 +1232,10 @@
       <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1256,10 +1256,10 @@
       <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1286,10 +1286,10 @@
       <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -1310,10 +1310,10 @@
       <c r="O3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1340,10 +1340,10 @@
       <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -1364,10 +1364,10 @@
       <c r="O4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1394,10 +1394,10 @@
       <c r="G5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>55</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -1418,10 +1418,10 @@
       <c r="O5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1880,7 +1880,7 @@
       <c r="G14" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>198</v>
       </c>
       <c r="I14" s="4" t="s">
@@ -1904,7 +1904,7 @@
       <c r="O14" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="P14" s="3" t="s">
         <v>206</v>
       </c>
       <c r="Q14" s="4" t="s">
@@ -1932,7 +1932,7 @@
       <c r="G15" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>213</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -1952,7 +1952,7 @@
         <v>218</v>
       </c>
       <c r="O15" s="3"/>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="3" t="s">
         <v>219</v>
       </c>
       <c r="Q15" s="4" t="s">
@@ -1978,7 +1978,7 @@
       <c r="G16" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>225</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -1996,7 +1996,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-      <c r="P16" s="4" t="s">
+      <c r="P16" s="3" t="s">
         <v>230</v>
       </c>
       <c r="Q16" s="4" t="s">
@@ -2024,7 +2024,7 @@
       <c r="G17" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>237</v>
       </c>
       <c r="I17" s="4" t="s">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="4" t="s">
+      <c r="P17" s="3" t="s">
         <v>243</v>
       </c>
       <c r="Q17" s="4" t="s">

</xml_diff>

<commit_message>
RST, LD NN SP, ADD SP N, LD HL SP N, ADD HL NN, JP HL, LD N16 A, LD A N16
</commit_message>
<xml_diff>
--- a/docs/Opcodes.xlsx
+++ b/docs/Opcodes.xlsx
@@ -797,7 +797,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,6 +808,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF395511"/>
         <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF706E0C"/>
+        <bgColor rgb="FF395511"/>
       </patternFill>
     </fill>
   </fills>
@@ -852,7 +858,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -870,10 +876,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,7 +913,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF706E0C"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -1133,7 +1143,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1238,10 +1248,10 @@
       <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1295,7 +1305,7 @@
       <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -1349,7 +1359,7 @@
       <c r="J4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1403,7 +1413,7 @@
       <c r="J5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>57</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1883,7 +1893,7 @@
       <c r="H14" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>199</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -1895,7 +1905,7 @@
       <c r="L14" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>203</v>
       </c>
       <c r="N14" s="3" t="s">
@@ -1907,7 +1917,7 @@
       <c r="P14" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="3" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1935,7 +1945,7 @@
       <c r="H15" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>214</v>
       </c>
       <c r="J15" s="3" t="s">
@@ -1955,7 +1965,7 @@
       <c r="P15" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="3" t="s">
         <v>220</v>
       </c>
     </row>
@@ -1981,16 +1991,16 @@
       <c r="H16" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="3" t="s">
         <v>229</v>
       </c>
       <c r="M16" s="3"/>
@@ -1999,7 +2009,7 @@
       <c r="P16" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="Q16" s="4" t="s">
+      <c r="Q16" s="3" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2027,16 +2037,16 @@
       <c r="H17" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="3" t="s">
         <v>241</v>
       </c>
       <c r="M17" s="3" t="s">
@@ -2047,7 +2057,7 @@
       <c r="P17" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="3" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2122,352 +2132,352 @@
         <f aca="false">DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A21)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A22)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A23)+16, 2)</f>
         <v>30</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A24)+16, 2)</f>
         <v>40</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A25)+16, 2)</f>
         <v>50</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A26)+16, 2)</f>
         <v>60</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A27)+16, 2)</f>
         <v>70</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A28)+16, 2)</f>
         <v>80</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A29)+16, 2)</f>
         <v>90</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A30)+16, 2)</f>
         <v>A0</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A31)+16, 2)</f>
         <v>B0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A32)+16, 2)</f>
         <v>C0</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A33)+16, 2)</f>
         <v>D0</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A34)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="str">
         <f aca="false">DEC2HEX(HEX2DEC(A35)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>